<commit_message>
I finished "Loyiha Ishi one"
I finished "Loyiha ishi one".
I added asset to my project.
</commit_message>
<xml_diff>
--- a/MBT/Assets/JobRanoOpa/PlayerPrefsLoyihaIshi.xlsx
+++ b/MBT/Assets/JobRanoOpa/PlayerPrefsLoyihaIshi.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>PlayerPrefslar</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>2.</t>
+  </si>
+  <si>
+    <t>"GraphicRasm5"</t>
   </si>
   <si>
     <t>3.</t>
@@ -78,14 +81,7 @@
     <numFmt numFmtId="178" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -541,148 +537,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1010,7 +1006,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="3"/>
@@ -1045,34 +1041,40 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>